<commit_message>
AutoCommit_15 декабря 2023 г. 12:38:28_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ДисМат_.xlsx
+++ b/2ИСИП-722_ДисМат_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>2ИСИП-722: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Дз8</t>
+  </si>
+  <si>
+    <t>м</t>
   </si>
 </sst>
 </file>
@@ -545,10 +548,10 @@
   <dimension ref="A1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
+      <selection pane="bottomRight" activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -784,7 +787,7 @@
     </row>
     <row r="5" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A34" si="2">IF(B5=C5,1+A4,"_______")</f>
+        <f t="shared" ref="A5:A33" si="2">IF(B5=C5,1+A4,"_______")</f>
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1404,12 +1407,24 @@
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5</v>
+      </c>
+      <c r="I14" s="5">
+        <v>5</v>
+      </c>
       <c r="J14" s="5">
         <v>5</v>
       </c>
@@ -2111,7 +2126,9 @@
       <c r="J24" s="5">
         <v>5</v>
       </c>
-      <c r="K24" s="5"/>
+      <c r="K24" s="5">
+        <v>5</v>
+      </c>
       <c r="L24" s="5">
         <v>2</v>
       </c>
@@ -2133,9 +2150,13 @@
       </c>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
+      <c r="S24" s="5">
+        <v>5</v>
+      </c>
       <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
+      <c r="U24" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 13:36:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ДисМат_.xlsx
+++ b/2ИСИП-722_ДисМат_.xlsx
@@ -548,10 +548,10 @@
   <dimension ref="A1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T4" sqref="T4"/>
+      <selection pane="bottomRight" activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1283,14 +1283,30 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
+        <v>5</v>
+      </c>
+      <c r="I12" s="5">
+        <v>5</v>
+      </c>
+      <c r="J12" s="5">
+        <v>5</v>
+      </c>
+      <c r="K12" s="5">
+        <v>10</v>
+      </c>
       <c r="L12" s="5">
         <v>3</v>
       </c>
@@ -1312,7 +1328,9 @@
       </c>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
+      <c r="S12" s="5">
+        <v>5</v>
+      </c>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
@@ -1472,7 +1490,9 @@
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="S14" s="5">
+        <v>5</v>
+      </c>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
@@ -2563,7 +2583,9 @@
       <c r="G30" s="5">
         <v>5</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="5">
+        <v>5</v>
+      </c>
       <c r="I30" s="5">
         <v>5</v>
       </c>
@@ -2594,7 +2616,9 @@
       </c>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
+      <c r="S30" s="5">
+        <v>4</v>
+      </c>
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
@@ -2709,8 +2733,12 @@
       <c r="I32" s="5">
         <v>5</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="J32" s="5">
+        <v>5</v>
+      </c>
+      <c r="K32" s="5">
+        <v>10</v>
+      </c>
       <c r="L32" s="5">
         <v>4</v>
       </c>
@@ -2732,7 +2760,9 @@
       </c>
       <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
+      <c r="S32" s="5">
+        <v>5</v>
+      </c>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>

</xml_diff>

<commit_message>
AutoCommit_19 декабря 2023 г. 16:08:03_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ДисМат_.xlsx
+++ b/2ИСИП-722_ДисМат_.xlsx
@@ -548,10 +548,10 @@
   <dimension ref="A1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
       </c>
       <c r="O3" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" si="0"/>
@@ -1082,15 +1082,33 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5">
+        <v>5</v>
+      </c>
+      <c r="I9" s="5">
+        <v>5</v>
+      </c>
+      <c r="J9" s="5">
+        <v>5</v>
+      </c>
+      <c r="K9" s="5">
+        <v>10</v>
+      </c>
+      <c r="L9" s="5">
+        <v>3</v>
+      </c>
       <c r="M9" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1101,7 +1119,7 @@
       </c>
       <c r="O9" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="5">
         <f t="shared" si="1"/>
@@ -1220,14 +1238,30 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5">
+        <v>5</v>
+      </c>
+      <c r="I11" s="5">
+        <v>5</v>
+      </c>
+      <c r="J11" s="5">
+        <v>5</v>
+      </c>
+      <c r="K11" s="5">
+        <v>10</v>
+      </c>
       <c r="L11" s="5">
         <v>3</v>
       </c>
@@ -1249,7 +1283,9 @@
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="S11" s="5">
+        <v>4</v>
+      </c>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
@@ -1526,13 +1562,27 @@
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5">
+        <v>5</v>
+      </c>
+      <c r="I15" s="5">
+        <v>5</v>
+      </c>
+      <c r="J15" s="5">
+        <v>5</v>
+      </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5">
         <v>3</v>
@@ -1555,7 +1605,9 @@
       </c>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+      <c r="S15" s="5">
+        <v>4</v>
+      </c>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
@@ -1713,7 +1765,9 @@
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+      <c r="S17" s="5">
+        <v>5</v>
+      </c>
       <c r="T17" s="5"/>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
@@ -2494,7 +2548,9 @@
       </c>
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
+      <c r="S28" s="5">
+        <v>4</v>
+      </c>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>

</xml_diff>

<commit_message>
AutoCommit_20 декабря 2023 г. 13:06:06_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ДисМат_.xlsx
+++ b/2ИСИП-722_ДисМат_.xlsx
@@ -551,7 +551,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S19" sqref="S19"/>
+      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1127,9 @@
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="S9" s="5">
+        <v>4</v>
+      </c>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>

</xml_diff>

<commit_message>
AutoCommit_23 декабря 2023 г. 9:57:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-722_ДисМат_.xlsx
+++ b/2ИСИП-722_ДисМат_.xlsx
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -250,6 +250,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -557,10 +560,10 @@
   <dimension ref="A1:AN42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -569,8 +572,9 @@
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="22.7265625" customWidth="1"/>
     <col min="4" max="11" width="2.90625" customWidth="1"/>
-    <col min="12" max="12" width="10.90625" customWidth="1"/>
-    <col min="13" max="24" width="3.81640625" customWidth="1"/>
+    <col min="12" max="12" width="4.08984375" customWidth="1"/>
+    <col min="13" max="13" width="8.54296875" customWidth="1"/>
+    <col min="14" max="24" width="3.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="15.5" x14ac:dyDescent="0.35">
@@ -639,22 +643,21 @@
       <c r="K2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>1</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>2</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>3</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>4</v>
       </c>
-      <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
@@ -691,24 +694,23 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4">
-        <f>SUM(M4:M33)</f>
-        <v>5</v>
-      </c>
+      <c r="M3" s="4"/>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:P3" si="0">SUM(N4:N33)</f>
+        <f>SUM(N4:N33)</f>
+        <v>5</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" ref="O3:Q3" si="0">SUM(O4:O33)</f>
         <v>6</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -768,31 +770,30 @@
       <c r="K4" s="5">
         <v>5</v>
       </c>
-      <c r="L4" s="5">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
-      <c r="M4" s="5">
-        <f t="shared" ref="M4:P33" si="1">IF($L4=M$2,1,0)</f>
-        <v>0</v>
-      </c>
       <c r="N4" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M4=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <f>IF($M4=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O4" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P4" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5"/>
+        <f>IF($M4=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>IF($M4=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R4" s="5"/>
-      <c r="S4" s="5">
-        <v>5</v>
-      </c>
-      <c r="T4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5">
+        <v>5</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -816,7 +817,7 @@
     </row>
     <row r="5" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A33" si="2">IF(B5=C5,1+A4,"_______")</f>
+        <f t="shared" ref="A5:A33" si="1">IF(B5=C5,1+A4,"_______")</f>
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -847,36 +848,38 @@
         <v>5</v>
       </c>
       <c r="K5" s="5">
-        <v>10</v>
-      </c>
-      <c r="L5" s="5">
+        <v>5</v>
+      </c>
+      <c r="L5" s="9">
+        <v>5</v>
+      </c>
+      <c r="M5" s="5">
         <v>4</v>
       </c>
-      <c r="M5" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N5" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M5=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M5=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P5" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M5=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5">
+        <f>IF($M5=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
-      <c r="S5" s="5">
-        <v>5</v>
-      </c>
-      <c r="T5" s="5" t="s">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
+        <v>5</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="U5" s="5"/>
       <c r="V5" s="5"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
@@ -899,7 +902,7 @@
     </row>
     <row r="6" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -916,34 +919,33 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>1</v>
       </c>
-      <c r="M6" s="5">
-        <f t="shared" si="1"/>
+      <c r="N6" s="5">
+        <f>IF($M6=N$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="N6" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="O6" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M6=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P6" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5"/>
+        <f>IF($M6=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5">
+        <f>IF($M6=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R6" s="5"/>
-      <c r="S6" s="5">
+      <c r="S6" s="5"/>
+      <c r="T6" s="5">
         <v>3</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="U6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U6" s="5"/>
       <c r="V6" s="5"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
@@ -966,7 +968,7 @@
     </row>
     <row r="7" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -983,34 +985,33 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5">
+      <c r="M7" s="5">
         <v>2</v>
       </c>
-      <c r="M7" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N7" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M7=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <f>IF($M7=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O7" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P7" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5"/>
+        <f>IF($M7=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="5">
+        <f>IF($M7=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R7" s="5"/>
-      <c r="S7" s="5">
+      <c r="S7" s="5"/>
+      <c r="T7" s="5">
         <v>3</v>
       </c>
-      <c r="T7" s="5" t="s">
+      <c r="U7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
@@ -1033,7 +1034,7 @@
     </row>
     <row r="8" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -1050,30 +1051,28 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="M8" s="5"/>
       <c r="N8" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M8=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M8=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5"/>
+        <f>IF($M8=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <f>IF($M8=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R8" s="5"/>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="5"/>
+      <c r="U8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
@@ -1096,7 +1095,7 @@
     </row>
     <row r="9" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B9" t="s">
@@ -1127,33 +1126,35 @@
         <v>5</v>
       </c>
       <c r="K9" s="5">
-        <v>10</v>
-      </c>
-      <c r="L9" s="5">
+        <v>5</v>
+      </c>
+      <c r="L9" s="9">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5">
         <v>3</v>
       </c>
-      <c r="M9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N9" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M9=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M9=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="5">
+        <f>IF($M9=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="5">
+        <f>IF($M9=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R9" s="5"/>
-      <c r="S9" s="5">
+      <c r="S9" s="5"/>
+      <c r="T9" s="5">
         <v>4</v>
       </c>
-      <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
@@ -1177,7 +1178,7 @@
     </row>
     <row r="10" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -1208,31 +1209,30 @@
         <v>5</v>
       </c>
       <c r="K10" s="5"/>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>1</v>
       </c>
-      <c r="M10" s="5">
-        <f t="shared" si="1"/>
+      <c r="N10" s="5">
+        <f>IF($M10=N$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="N10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="O10" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M10=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P10" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5"/>
+        <f>IF($M10=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="5">
+        <f>IF($M10=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R10" s="5"/>
-      <c r="S10" s="5">
+      <c r="S10" s="5"/>
+      <c r="T10" s="5">
         <v>4</v>
       </c>
-      <c r="T10" s="5"/>
       <c r="U10" s="5"/>
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="11" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B11" t="s">
@@ -1287,33 +1287,35 @@
         <v>5</v>
       </c>
       <c r="K11" s="5">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5">
+        <v>5</v>
+      </c>
+      <c r="L11" s="9">
+        <v>5</v>
+      </c>
+      <c r="M11" s="5">
         <v>3</v>
       </c>
-      <c r="M11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N11" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M11=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M11=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="5">
+        <f>IF($M11=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P11" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5"/>
+      <c r="Q11" s="5">
+        <f>IF($M11=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R11" s="5"/>
-      <c r="S11" s="5">
+      <c r="S11" s="5"/>
+      <c r="T11" s="5">
         <v>4</v>
       </c>
-      <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
@@ -1337,7 +1339,7 @@
     </row>
     <row r="12" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B12" t="s">
@@ -1368,33 +1370,35 @@
         <v>5</v>
       </c>
       <c r="K12" s="5">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5">
+        <v>5</v>
+      </c>
+      <c r="L12" s="9">
+        <v>5</v>
+      </c>
+      <c r="M12" s="5">
         <v>3</v>
       </c>
-      <c r="M12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N12" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M12=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M12=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <f>IF($M12=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P12" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="5"/>
+      <c r="Q12" s="5">
+        <f>IF($M12=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R12" s="5"/>
-      <c r="S12" s="5">
-        <v>5</v>
-      </c>
-      <c r="T12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5">
+        <v>5</v>
+      </c>
       <c r="U12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
@@ -1418,7 +1422,7 @@
     </row>
     <row r="13" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B13" t="s">
@@ -1449,33 +1453,35 @@
         <v>5</v>
       </c>
       <c r="K13" s="5">
-        <v>10</v>
-      </c>
-      <c r="L13" s="5">
+        <v>5</v>
+      </c>
+      <c r="L13" s="9">
+        <v>5</v>
+      </c>
+      <c r="M13" s="5">
         <v>4</v>
       </c>
-      <c r="M13" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N13" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M13=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M13=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P13" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M13=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="5">
+        <f>IF($M13=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="5">
-        <v>5</v>
-      </c>
-      <c r="T13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5">
+        <v>5</v>
+      </c>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
@@ -1499,7 +1505,7 @@
     </row>
     <row r="14" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B14" t="s">
@@ -1532,31 +1538,30 @@
       <c r="K14" s="5">
         <v>5</v>
       </c>
-      <c r="L14" s="5">
+      <c r="M14" s="5">
         <v>3</v>
       </c>
-      <c r="M14" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N14" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M14=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M14=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <f>IF($M14=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P14" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5"/>
+      <c r="Q14" s="5">
+        <f>IF($M14=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R14" s="5"/>
-      <c r="S14" s="5">
-        <v>5</v>
-      </c>
-      <c r="T14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5">
+        <v>5</v>
+      </c>
       <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
@@ -1580,7 +1585,7 @@
     </row>
     <row r="15" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B15" t="s">
@@ -1611,31 +1616,30 @@
         <v>5</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="5">
+      <c r="M15" s="5">
         <v>3</v>
       </c>
-      <c r="M15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N15" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M15=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M15=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <f>IF($M15=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P15" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5"/>
+      <c r="Q15" s="5">
+        <f>IF($M15=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R15" s="5"/>
-      <c r="S15" s="5">
+      <c r="S15" s="5"/>
+      <c r="T15" s="5">
         <v>4</v>
       </c>
-      <c r="T15" s="5"/>
       <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
@@ -1659,7 +1663,7 @@
     </row>
     <row r="16" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B16" t="s">
@@ -1692,29 +1696,28 @@
       <c r="K16" s="5">
         <v>5</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="M16" s="5"/>
       <c r="N16" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M16=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M16=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P16" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="5"/>
+        <f>IF($M16=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="5">
+        <f>IF($M16=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R16" s="5"/>
-      <c r="S16" s="5">
+      <c r="S16" s="5"/>
+      <c r="T16" s="5">
         <v>4</v>
       </c>
-      <c r="T16" s="5"/>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
@@ -1738,7 +1741,7 @@
     </row>
     <row r="17" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B17" t="s">
@@ -1769,33 +1772,35 @@
         <v>5</v>
       </c>
       <c r="K17" s="5">
-        <v>10</v>
-      </c>
-      <c r="L17" s="5">
+        <v>5</v>
+      </c>
+      <c r="L17" s="9">
+        <v>5</v>
+      </c>
+      <c r="M17" s="5">
         <v>1</v>
       </c>
-      <c r="M17" s="5">
-        <f t="shared" si="1"/>
+      <c r="N17" s="5">
+        <f>IF($M17=N$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="N17" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="O17" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M17=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P17" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="5"/>
+        <f>IF($M17=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="5">
+        <f>IF($M17=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R17" s="5"/>
-      <c r="S17" s="5">
-        <v>5</v>
-      </c>
-      <c r="T17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5">
+        <v>5</v>
+      </c>
       <c r="U17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
@@ -1819,7 +1824,7 @@
     </row>
     <row r="18" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B18" t="s">
@@ -1836,32 +1841,31 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="M18" s="5"/>
       <c r="N18" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M18=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M18=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P18" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="5"/>
+        <f>IF($M18=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="5">
+        <f>IF($M18=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R18" s="5"/>
-      <c r="S18" s="5">
+      <c r="S18" s="5"/>
+      <c r="T18" s="5">
         <v>3</v>
       </c>
-      <c r="T18" s="5" t="s">
+      <c r="U18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
@@ -1884,7 +1888,7 @@
     </row>
     <row r="19" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B19" t="s">
@@ -1915,33 +1919,35 @@
         <v>5</v>
       </c>
       <c r="K19" s="5">
-        <v>10</v>
-      </c>
-      <c r="L19" s="5">
+        <v>5</v>
+      </c>
+      <c r="L19" s="9">
+        <v>5</v>
+      </c>
+      <c r="M19" s="5">
         <v>2</v>
       </c>
-      <c r="M19" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N19" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M19=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="5">
+        <f>IF($M19=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O19" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P19" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="5"/>
+        <f>IF($M19=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="5">
+        <f>IF($M19=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R19" s="5"/>
-      <c r="S19" s="5">
-        <v>5</v>
-      </c>
-      <c r="T19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5">
+        <v>5</v>
+      </c>
       <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
@@ -1965,7 +1971,7 @@
     </row>
     <row r="20" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B20" t="s">
@@ -1996,33 +2002,35 @@
         <v>5</v>
       </c>
       <c r="K20" s="5">
-        <v>10</v>
-      </c>
-      <c r="L20" s="5">
+        <v>5</v>
+      </c>
+      <c r="L20" s="9">
+        <v>5</v>
+      </c>
+      <c r="M20" s="5">
         <v>2</v>
       </c>
-      <c r="M20" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N20" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M20=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20" s="5">
+        <f>IF($M20=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O20" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P20" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="5"/>
+        <f>IF($M20=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="5">
+        <f>IF($M20=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R20" s="5"/>
-      <c r="S20" s="5">
-        <v>5</v>
-      </c>
-      <c r="T20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5">
+        <v>5</v>
+      </c>
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
@@ -2046,7 +2054,7 @@
     </row>
     <row r="21" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B21" t="s">
@@ -2079,31 +2087,30 @@
       <c r="K21" s="5">
         <v>5</v>
       </c>
-      <c r="L21" s="5">
+      <c r="M21" s="5">
         <v>4</v>
       </c>
-      <c r="M21" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N21" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M21=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M21=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P21" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M21=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
+        <f>IF($M21=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
-      <c r="S21" s="5">
-        <v>5</v>
-      </c>
-      <c r="T21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5">
+        <v>5</v>
+      </c>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
@@ -2127,7 +2134,7 @@
     </row>
     <row r="22" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B22" t="s">
@@ -2144,32 +2151,31 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="M22" s="5"/>
       <c r="N22" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M22=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M22=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P22" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="5"/>
+        <f>IF($M22=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="5">
+        <f>IF($M22=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R22" s="5"/>
-      <c r="S22" s="5">
+      <c r="S22" s="5"/>
+      <c r="T22" s="5">
         <v>4</v>
       </c>
-      <c r="T22" s="5" t="s">
+      <c r="U22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U22" s="5"/>
       <c r="V22" s="5"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="23" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B23" t="s">
@@ -2209,34 +2215,33 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5">
+      <c r="M23" s="5">
         <v>2</v>
       </c>
-      <c r="M23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N23" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M23=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="5">
+        <f>IF($M23=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P23" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="5"/>
+        <f>IF($M23=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="5">
+        <f>IF($M23=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R23" s="5"/>
-      <c r="S23" s="5">
+      <c r="S23" s="5"/>
+      <c r="T23" s="5">
         <v>3</v>
       </c>
-      <c r="T23" s="5" t="s">
+      <c r="U23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U23" s="5"/>
       <c r="V23" s="5"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
@@ -2259,7 +2264,7 @@
     </row>
     <row r="24" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B24" t="s">
@@ -2292,35 +2297,34 @@
       <c r="K24" s="5">
         <v>5</v>
       </c>
-      <c r="L24" s="5">
+      <c r="M24" s="5">
         <v>2</v>
       </c>
-      <c r="M24" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N24" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M24=N$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="5">
+        <f>IF($M24=O$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="O24" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="P24" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="5"/>
+        <f>IF($M24=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="5">
+        <f>IF($M24=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R24" s="5"/>
-      <c r="S24" s="5">
-        <v>5</v>
-      </c>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5" t="s">
+      <c r="S24" s="5"/>
+      <c r="T24" s="5">
+        <v>5</v>
+      </c>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="V24" s="5"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="3"/>
@@ -2342,7 +2346,7 @@
     </row>
     <row r="25" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B25" t="s">
@@ -2373,33 +2377,35 @@
         <v>5</v>
       </c>
       <c r="K25" s="5">
-        <v>10</v>
-      </c>
-      <c r="L25" s="5">
+        <v>5</v>
+      </c>
+      <c r="L25" s="9">
+        <v>5</v>
+      </c>
+      <c r="M25" s="5">
         <v>4</v>
       </c>
-      <c r="M25" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N25" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M25=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M25=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M25=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="5">
+        <f>IF($M25=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q25" s="5"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="5">
-        <v>5</v>
-      </c>
-      <c r="T25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5">
+        <v>5</v>
+      </c>
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
@@ -2423,7 +2429,7 @@
     </row>
     <row r="26" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B26" t="s">
@@ -2454,33 +2460,35 @@
         <v>5</v>
       </c>
       <c r="K26" s="5">
-        <v>10</v>
-      </c>
-      <c r="L26" s="5">
+        <v>5</v>
+      </c>
+      <c r="L26" s="9">
+        <v>5</v>
+      </c>
+      <c r="M26" s="5">
         <v>4</v>
       </c>
-      <c r="M26" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N26" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M26=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M26=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P26" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M26=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="5">
+        <f>IF($M26=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q26" s="5"/>
       <c r="R26" s="5"/>
-      <c r="S26" s="5">
+      <c r="S26" s="5"/>
+      <c r="T26" s="5">
         <v>4</v>
       </c>
-      <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
@@ -2504,7 +2512,7 @@
     </row>
     <row r="27" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B27" t="s">
@@ -2537,31 +2545,30 @@
       <c r="K27" s="5">
         <v>5</v>
       </c>
-      <c r="L27" s="5">
+      <c r="M27" s="5">
         <v>4</v>
       </c>
-      <c r="M27" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N27" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M27=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O27" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M27=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P27" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M27=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="5">
+        <f>IF($M27=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q27" s="5"/>
       <c r="R27" s="5"/>
-      <c r="S27" s="5">
+      <c r="S27" s="5"/>
+      <c r="T27" s="5">
         <v>3</v>
       </c>
-      <c r="T27" s="5"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
@@ -2585,7 +2592,7 @@
     </row>
     <row r="28" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B28" t="s">
@@ -2614,31 +2621,30 @@
         <v>5</v>
       </c>
       <c r="K28" s="5"/>
-      <c r="L28" s="5">
+      <c r="M28" s="5">
         <v>1</v>
       </c>
-      <c r="M28" s="5">
-        <f t="shared" si="1"/>
+      <c r="N28" s="5">
+        <f>IF($M28=N$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="N28" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="O28" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M28=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P28" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="5"/>
+        <f>IF($M28=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="5">
+        <f>IF($M28=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R28" s="5"/>
-      <c r="S28" s="5">
+      <c r="S28" s="5"/>
+      <c r="T28" s="5">
         <v>4</v>
       </c>
-      <c r="T28" s="5"/>
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
@@ -2662,7 +2668,7 @@
     </row>
     <row r="29" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B29" t="s">
@@ -2679,31 +2685,30 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
-      <c r="L29" s="5">
+      <c r="M29" s="5">
         <v>1</v>
       </c>
-      <c r="M29" s="5">
-        <f t="shared" si="1"/>
+      <c r="N29" s="5">
+        <f>IF($M29=N$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="N29" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="O29" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M29=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P29" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="5"/>
+        <f>IF($M29=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5">
+        <f>IF($M29=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R29" s="5"/>
-      <c r="S29" s="5">
+      <c r="S29" s="5"/>
+      <c r="T29" s="5">
         <v>3</v>
       </c>
-      <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
@@ -2727,7 +2732,7 @@
     </row>
     <row r="30" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -2760,31 +2765,30 @@
       <c r="K30" s="5">
         <v>5</v>
       </c>
-      <c r="L30" s="5">
+      <c r="M30" s="5">
         <v>4</v>
       </c>
-      <c r="M30" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N30" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M30=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M30=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P30" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M30=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="5">
+        <f>IF($M30=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-      <c r="S30" s="5">
+      <c r="S30" s="5"/>
+      <c r="T30" s="5">
         <v>4</v>
       </c>
-      <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
@@ -2808,7 +2812,7 @@
     </row>
     <row r="31" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -2825,34 +2829,33 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
-      <c r="L31" s="5">
+      <c r="M31" s="5">
         <v>3</v>
       </c>
-      <c r="M31" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N31" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M31=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M31=O$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="5">
+        <f>IF($M31=P$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P31" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="5"/>
+      <c r="Q31" s="5">
+        <f>IF($M31=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R31" s="5"/>
-      <c r="S31" s="5">
+      <c r="S31" s="5"/>
+      <c r="T31" s="5">
         <v>3</v>
       </c>
-      <c r="T31" s="5" t="s">
+      <c r="U31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
@@ -2875,7 +2878,7 @@
     </row>
     <row r="32" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -2906,33 +2909,35 @@
         <v>5</v>
       </c>
       <c r="K32" s="5">
-        <v>10</v>
-      </c>
-      <c r="L32" s="5">
+        <v>5</v>
+      </c>
+      <c r="L32" s="9">
+        <v>5</v>
+      </c>
+      <c r="M32" s="5">
         <v>4</v>
       </c>
-      <c r="M32" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
       <c r="N32" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M32=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M32=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P32" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M32=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="5">
+        <f>IF($M32=Q$2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q32" s="5"/>
       <c r="R32" s="5"/>
-      <c r="S32" s="5">
-        <v>5</v>
-      </c>
-      <c r="T32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5">
+        <v>5</v>
+      </c>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
@@ -2956,7 +2961,7 @@
     </row>
     <row r="33" spans="1:40" ht="12" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B33" t="s">
@@ -2973,32 +2978,31 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="M33" s="5"/>
       <c r="N33" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M33=N$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="1"/>
+        <f>IF($M33=O$2,1,0)</f>
         <v>0</v>
       </c>
       <c r="P33" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="5"/>
+        <f>IF($M33=P$2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="5">
+        <f>IF($M33=Q$2,1,0)</f>
+        <v>0</v>
+      </c>
       <c r="R33" s="5"/>
-      <c r="S33" s="5">
+      <c r="S33" s="5"/>
+      <c r="T33" s="5">
         <v>4</v>
       </c>
-      <c r="T33" s="5" t="s">
+      <c r="U33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
       <c r="X33" s="5"/>
@@ -3029,7 +3033,6 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
@@ -3068,7 +3071,6 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
@@ -3107,7 +3109,6 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
@@ -3146,7 +3147,6 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
@@ -3185,7 +3185,6 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>

</xml_diff>